<commit_message>
Création du dictionnaire de données
</commit_message>
<xml_diff>
--- a/Dictionnaire de Donné cardgame.xlsx
+++ b/Dictionnaire de Donné cardgame.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stagiaire\Documents\GitHub\whinners_cardgame\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E5D9419-336E-4AD2-B011-41745871E4E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9604484-92EA-42BE-9BA7-A7C05F2195E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="360" windowWidth="25440" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="60">
   <si>
     <t>Mnémonique</t>
   </si>
@@ -193,13 +193,25 @@
   </si>
   <si>
     <t>B</t>
+  </si>
+  <si>
+    <t>card_id</t>
+  </si>
+  <si>
+    <t>Identifiant de la carte dans le programme.</t>
+  </si>
+  <si>
+    <t>creature_id</t>
+  </si>
+  <si>
+    <t>Identifiant de la créature dans le système</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -217,6 +229,22 @@
     <font>
       <sz val="16"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -242,7 +270,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -255,6 +283,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -269,21 +303,6 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
         <color theme="1"/>
         <name val="Calibri"/>
         <family val="2"/>
@@ -366,6 +385,21 @@
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -380,14 +414,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{56DE3692-9790-4744-A789-3E6055E4AC06}" name="Tableau1" displayName="Tableau1" ref="A1:E1048568" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
-  <autoFilter ref="A1:E1048568" xr:uid="{56DE3692-9790-4744-A789-3E6055E4AC06}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{56DE3692-9790-4744-A789-3E6055E4AC06}" name="Tableau1" displayName="Tableau1" ref="A1:E1048566" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A1:E1048566" xr:uid="{56DE3692-9790-4744-A789-3E6055E4AC06}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{8EBB0957-8234-41ED-BA5C-E96FB87927FE}" name="Mnémonique" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{164577FC-C01A-4834-8BF7-A1E0D1350250}" name="Signification" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{B948BAF6-1637-44C3-A1D7-0802A11BA100}" name="Type" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{A242C56C-2355-40B7-B867-2F0695C76037}" name="Longueur" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{4CEB66E1-1BF7-4FE3-AA78-8BD626D1CAC0}" name="Contrainte" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{8EBB0957-8234-41ED-BA5C-E96FB87927FE}" name="Mnémonique" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{164577FC-C01A-4834-8BF7-A1E0D1350250}" name="Signification" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{B948BAF6-1637-44C3-A1D7-0802A11BA100}" name="Type" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{A242C56C-2355-40B7-B867-2F0695C76037}" name="Longueur" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{4CEB66E1-1BF7-4FE3-AA78-8BD626D1CAC0}" name="Contrainte" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -656,11 +690,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B29" sqref="B29"/>
+      <selection pane="bottomLeft" activeCell="A20" sqref="A20:XFD20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -691,16 +725,19 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="D2" s="6">
+        <v>48</v>
+      </c>
+      <c r="E2" s="6" t="s">
         <v>49</v>
       </c>
     </row>
@@ -714,6 +751,9 @@
       <c r="C3" s="3" t="s">
         <v>52</v>
       </c>
+      <c r="D3" s="3">
+        <v>48</v>
+      </c>
       <c r="E3" s="3" t="s">
         <v>20</v>
       </c>
@@ -728,6 +768,9 @@
       <c r="C4" s="3" t="s">
         <v>52</v>
       </c>
+      <c r="D4" s="3">
+        <v>48</v>
+      </c>
       <c r="E4" s="3" t="s">
         <v>20</v>
       </c>
@@ -742,33 +785,39 @@
       <c r="C5" s="3" t="s">
         <v>54</v>
       </c>
+      <c r="D5" s="3">
+        <v>48</v>
+      </c>
       <c r="E5" s="3" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="5" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="5">
         <v>11</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -784,6 +833,26 @@
       <c r="D8" s="3">
         <v>11</v>
       </c>
+      <c r="E8" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" s="6">
+        <v>11</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
@@ -795,15 +864,21 @@
       <c r="C10" s="3" t="s">
         <v>52</v>
       </c>
+      <c r="D10" s="3">
+        <v>48</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="5" t="s">
         <v>54</v>
       </c>
     </row>
@@ -817,164 +892,205 @@
       <c r="C12" s="3" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="D12" s="3">
+        <v>255</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D13" s="6">
+        <v>11</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D14" s="3">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>49</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>52</v>
+        <v>54</v>
+      </c>
+      <c r="D15" s="3">
+        <v>255</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>20</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C16" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D16" s="3">
+        <v>16</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D17" s="6">
+        <v>11</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="E16" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>20</v>
+      <c r="D18" s="5">
+        <v>96</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D19" s="3">
-        <v>11</v>
+        <v>55</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>55</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C23" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="E23" s="3" t="s">
+      <c r="E22" s="3" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D23" s="6">
+        <v>11</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
+      </c>
+      <c r="D24" s="3">
+        <v>4</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C26" s="3" t="s">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C25" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="E26" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E27" s="3" t="s">
+      <c r="D25" s="3">
+        <v>4</v>
+      </c>
+      <c r="E25" s="3" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>